<commit_message>
Reportes obtenidos y marca si esta vacio o no
</commit_message>
<xml_diff>
--- a/data/input/Deudas/Anticipos - BIANCOTTI, Nicols.xlsx
+++ b/data/input/Deudas/Anticipos - BIANCOTTI, Nicols.xlsx
@@ -61,13 +61,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -487,42 +484,30 @@
     <row r="3"/>
     <row r="4"/>
     <row r="5"/>
-    <row r="6">
-      <c r="A6" s="2" t="n"/>
-      <c r="B6" s="2" t="n"/>
-      <c r="C6" s="2" t="n"/>
-      <c r="D6" s="2" t="n"/>
-      <c r="E6" s="2" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
-      <c r="C7" s="2" t="n"/>
-      <c r="D7" s="2" t="n"/>
-      <c r="E7" s="2" t="n"/>
-    </row>
+    <row r="6"/>
+    <row r="7"/>
     <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Impuesto</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>Ant. / Cuota</t>
         </is>
       </c>
-      <c r="C8" s="3" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>Período Fiscal</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>Fecha de Vencimiento</t>
         </is>
       </c>
-      <c r="E8" s="3" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>Saldo</t>
         </is>

</xml_diff>